<commit_message>
api token and value code changes
</commit_message>
<xml_diff>
--- a/src/assets/ApiTestReport.xlsx
+++ b/src/assets/ApiTestReport.xlsx
@@ -463,7 +463,7 @@
         <v>/user/getUser</v>
       </c>
       <c r="G2" t="str">
-        <v>{"userID":"353"}</v>
+        <v>{"userID":"670"}</v>
       </c>
       <c r="I2" t="str">
         <v>200</v>
@@ -480,16 +480,16 @@
         <v>com.hashedin.broadcast.autotest.JarTest</v>
       </c>
       <c r="B3" t="str">
-        <v>PUT</v>
+        <v>POST</v>
       </c>
       <c r="C3" t="str">
         <v>http://localhost:8095/v3/api-docs</v>
       </c>
       <c r="D3" t="str">
-        <v>/user/updateUser</v>
+        <v>/user/createUser</v>
       </c>
       <c r="E3" t="str">
-        <v>{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"}</v>
+        <v>{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"}</v>
       </c>
       <c r="I3" t="str">
         <v>200</v>
@@ -509,16 +509,13 @@
         <v>com.hashedin.broadcast.autotest.JarTest</v>
       </c>
       <c r="B4" t="str">
-        <v>DELETE</v>
+        <v>GET</v>
       </c>
       <c r="C4" t="str">
         <v>http://localhost:8095/v3/api-docs</v>
       </c>
       <c r="D4" t="str">
-        <v>/user/deleteUser</v>
-      </c>
-      <c r="G4" t="str">
-        <v>{"userID":"353"}</v>
+        <v>/user/getUsers</v>
       </c>
       <c r="I4" t="str">
         <v>200</v>
@@ -535,16 +532,16 @@
         <v>com.hashedin.broadcast.autotest.JarTest</v>
       </c>
       <c r="B5" t="str">
-        <v>POST</v>
+        <v>PUT</v>
       </c>
       <c r="C5" t="str">
         <v>http://localhost:8095/v3/api-docs</v>
       </c>
       <c r="D5" t="str">
-        <v>/user/createUser</v>
+        <v>/user/updateUser</v>
       </c>
       <c r="E5" t="str">
-        <v>{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"}</v>
+        <v>{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"}</v>
       </c>
       <c r="I5" t="str">
         <v>200</v>
@@ -564,13 +561,16 @@
         <v>com.hashedin.broadcast.autotest.JarTest</v>
       </c>
       <c r="B6" t="str">
-        <v>GET</v>
+        <v>DELETE</v>
       </c>
       <c r="C6" t="str">
         <v>http://localhost:8095/v3/api-docs</v>
       </c>
       <c r="D6" t="str">
-        <v>/user/getUsers</v>
+        <v>/user/deleteUser</v>
+      </c>
+      <c r="G6" t="str">
+        <v>{"userID":"670"}</v>
       </c>
       <c r="I6" t="str">
         <v>200</v>
@@ -619,7 +619,7 @@
         <v>/action/createAction</v>
       </c>
       <c r="E8" t="str">
-        <v>{"updatedBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"createdBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"actionID":"697","description":"E9DdU","projectID":{"updatedBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"createdBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"description":"y2Rmj","projectName":"sF4pm","projectID":"210"},"actionName":"FDhBP"}</v>
+        <v>{"updatedBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"createdBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"actionID":"476","description":"aKlOb","projectID":{"updatedBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"createdBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"description":"5rGdL","projectName":"0NwWb","projectID":"198"},"actionName":"hp0RM"}</v>
       </c>
       <c r="I8" t="str">
         <v>200</v>
@@ -648,7 +648,7 @@
         <v>/action/updateAction</v>
       </c>
       <c r="E9" t="str">
-        <v>{"updatedBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"createdBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"actionID":"697","description":"E9DdU","projectID":{"updatedBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"createdBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"description":"y2Rmj","projectName":"sF4pm","projectID":"210"},"actionName":"FDhBP"}</v>
+        <v>{"updatedBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"createdBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"actionID":"476","description":"aKlOb","projectID":{"updatedBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"createdBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"description":"5rGdL","projectName":"0NwWb","projectID":"198"},"actionName":"hp0RM"}</v>
       </c>
       <c r="I9" t="str">
         <v>200</v>
@@ -677,7 +677,7 @@
         <v>/action/deleteAction</v>
       </c>
       <c r="G10" t="str">
-        <v>{"actionID":"697"}</v>
+        <v>{"actionID":"476"}</v>
       </c>
       <c r="I10" t="str">
         <v>200</v>
@@ -703,7 +703,7 @@
         <v>/action/getAction</v>
       </c>
       <c r="G11" t="str">
-        <v>{"actionID":"697"}</v>
+        <v>{"actionID":"476"}</v>
       </c>
       <c r="I11" t="str">
         <v>200</v>
@@ -752,7 +752,7 @@
         <v>/project/createProject</v>
       </c>
       <c r="E13" t="str">
-        <v>{"updatedBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"createdBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"description":"y2Rmj","projectName":"sF4pm","projectID":"210"}</v>
+        <v>{"updatedBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"createdBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"description":"5rGdL","projectName":"0NwWb","projectID":"198"}</v>
       </c>
       <c r="I13" t="str">
         <v>200</v>
@@ -772,25 +772,22 @@
         <v>com.hashedin.broadcast.autotest.JarTest</v>
       </c>
       <c r="B14" t="str">
-        <v>PUT</v>
+        <v>DELETE</v>
       </c>
       <c r="C14" t="str">
         <v>http://localhost:8095/v3/api-docs</v>
       </c>
       <c r="D14" t="str">
-        <v>/project/updateProject</v>
-      </c>
-      <c r="E14" t="str">
-        <v>{"updatedBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"createdBy":{"firstName":"BCaJe","lastName":"K2iT5","emailID":"qpL5w","userID":"353"},"description":"y2Rmj","projectName":"sF4pm","projectID":"210"}</v>
+        <v>/project/deleteProject</v>
+      </c>
+      <c r="G14" t="str">
+        <v>{"projectID":"198"}</v>
       </c>
       <c r="I14" t="str">
         <v>200</v>
       </c>
       <c r="M14" t="str">
         <v>{"Content-Type":"application/json"}</v>
-      </c>
-      <c r="N14" t="str">
-        <v>Project</v>
       </c>
       <c r="O14" t="str">
         <v>ProjectController</v>
@@ -801,22 +798,25 @@
         <v>com.hashedin.broadcast.autotest.JarTest</v>
       </c>
       <c r="B15" t="str">
-        <v>DELETE</v>
+        <v>PUT</v>
       </c>
       <c r="C15" t="str">
         <v>http://localhost:8095/v3/api-docs</v>
       </c>
       <c r="D15" t="str">
-        <v>/project/deleteProject</v>
-      </c>
-      <c r="G15" t="str">
-        <v>{"projectID":"210"}</v>
+        <v>/project/updateProject</v>
+      </c>
+      <c r="E15" t="str">
+        <v>{"updatedBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"createdBy":{"firstName":"RE8hP","lastName":"9k60a","emailID":"jESW3","userID":"670"},"description":"5rGdL","projectName":"0NwWb","projectID":"198"}</v>
       </c>
       <c r="I15" t="str">
         <v>200</v>
       </c>
       <c r="M15" t="str">
         <v>{"Content-Type":"application/json"}</v>
+      </c>
+      <c r="N15" t="str">
+        <v>Project</v>
       </c>
       <c r="O15" t="str">
         <v>ProjectController</v>
@@ -836,7 +836,7 @@
         <v>/project/getProject/{projectID}</v>
       </c>
       <c r="F16" t="str">
-        <v>{"projectID":"210"}</v>
+        <v>{"projectID":"198"}</v>
       </c>
       <c r="I16" t="str">
         <v>200</v>

</xml_diff>